<commit_message>
local ssh_wsl port forward
</commit_message>
<xml_diff>
--- a/python_ex/forEn.xlsx
+++ b/python_ex/forEn.xlsx
@@ -4412,7 +4412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2276"/>
+  <dimension ref="A1:F2396"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
@@ -72617,6 +72617,3606 @@
       <c r="F2276" t="inlineStr">
         <is>
           <t>2022-11-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2277">
+      <c r="A2277" t="inlineStr">
+        <is>
+          <t>TIGER TOP10</t>
+        </is>
+      </c>
+      <c r="B2277" t="inlineStr">
+        <is>
+          <t>72,835</t>
+        </is>
+      </c>
+      <c r="C2277" t="inlineStr">
+        <is>
+          <t>7,102</t>
+        </is>
+      </c>
+      <c r="D2277" t="inlineStr">
+        <is>
+          <t>-0.44%</t>
+        </is>
+      </c>
+      <c r="E2277" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2277" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2278">
+      <c r="A2278" t="inlineStr">
+        <is>
+          <t>NAVER</t>
+        </is>
+      </c>
+      <c r="B2278" t="inlineStr">
+        <is>
+          <t>43,505</t>
+        </is>
+      </c>
+      <c r="C2278" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+      <c r="D2278" t="inlineStr">
+        <is>
+          <t>-0.28%</t>
+        </is>
+      </c>
+      <c r="E2278" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2278" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2279">
+      <c r="A2279" t="inlineStr">
+        <is>
+          <t>삼성전기</t>
+        </is>
+      </c>
+      <c r="B2279" t="inlineStr">
+        <is>
+          <t>72,439</t>
+        </is>
+      </c>
+      <c r="C2279" t="inlineStr">
+        <is>
+          <t>531</t>
+        </is>
+      </c>
+      <c r="D2279" t="inlineStr">
+        <is>
+          <t>-0.36%</t>
+        </is>
+      </c>
+      <c r="E2279" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2279" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2280">
+      <c r="A2280" t="inlineStr">
+        <is>
+          <t>POSCO홀딩스</t>
+        </is>
+      </c>
+      <c r="B2280" t="inlineStr">
+        <is>
+          <t>34,874</t>
+        </is>
+      </c>
+      <c r="C2280" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="D2280" t="inlineStr">
+        <is>
+          <t>+0.18%</t>
+        </is>
+      </c>
+      <c r="E2280" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2280" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2281">
+      <c r="A2281" t="inlineStr">
+        <is>
+          <t>SK하이닉스</t>
+        </is>
+      </c>
+      <c r="B2281" t="inlineStr">
+        <is>
+          <t>49,812</t>
+        </is>
+      </c>
+      <c r="C2281" t="inlineStr">
+        <is>
+          <t>561</t>
+        </is>
+      </c>
+      <c r="D2281" t="inlineStr">
+        <is>
+          <t>+1.12%</t>
+        </is>
+      </c>
+      <c r="E2281" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2281" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2282">
+      <c r="A2282" t="inlineStr">
+        <is>
+          <t>KODEX 200선물인버스2X</t>
+        </is>
+      </c>
+      <c r="B2282" t="inlineStr">
+        <is>
+          <t>27,142</t>
+        </is>
+      </c>
+      <c r="C2282" t="inlineStr">
+        <is>
+          <t>8,789</t>
+        </is>
+      </c>
+      <c r="D2282" t="inlineStr">
+        <is>
+          <t>+0.16%</t>
+        </is>
+      </c>
+      <c r="E2282" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2282" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2283">
+      <c r="A2283" t="inlineStr">
+        <is>
+          <t>LG에너지솔루션</t>
+        </is>
+      </c>
+      <c r="B2283" t="inlineStr">
+        <is>
+          <t>47,854</t>
+        </is>
+      </c>
+      <c r="C2283" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="D2283" t="inlineStr">
+        <is>
+          <t>+1.84%</t>
+        </is>
+      </c>
+      <c r="E2283" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2283" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2284">
+      <c r="A2284" t="inlineStr">
+        <is>
+          <t>카카오페이</t>
+        </is>
+      </c>
+      <c r="B2284" t="inlineStr">
+        <is>
+          <t>23,387</t>
+        </is>
+      </c>
+      <c r="C2284" t="inlineStr">
+        <is>
+          <t>495</t>
+        </is>
+      </c>
+      <c r="D2284" t="inlineStr">
+        <is>
+          <t>-4.02%</t>
+        </is>
+      </c>
+      <c r="E2284" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2284" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2285">
+      <c r="A2285" t="inlineStr">
+        <is>
+          <t>금양</t>
+        </is>
+      </c>
+      <c r="B2285" t="inlineStr">
+        <is>
+          <t>31,668</t>
+        </is>
+      </c>
+      <c r="C2285" t="inlineStr">
+        <is>
+          <t>848</t>
+        </is>
+      </c>
+      <c r="D2285" t="inlineStr">
+        <is>
+          <t>-9.23%</t>
+        </is>
+      </c>
+      <c r="E2285" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2285" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2286">
+      <c r="A2286" t="inlineStr">
+        <is>
+          <t>카카오</t>
+        </is>
+      </c>
+      <c r="B2286" t="inlineStr">
+        <is>
+          <t>19,962</t>
+        </is>
+      </c>
+      <c r="C2286" t="inlineStr">
+        <is>
+          <t>378</t>
+        </is>
+      </c>
+      <c r="D2286" t="inlineStr">
+        <is>
+          <t>-0.77%</t>
+        </is>
+      </c>
+      <c r="E2286" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2286" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2287">
+      <c r="A2287" t="inlineStr">
+        <is>
+          <t>삼성SDI</t>
+        </is>
+      </c>
+      <c r="B2287" t="inlineStr">
+        <is>
+          <t>26,354</t>
+        </is>
+      </c>
+      <c r="C2287" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="D2287" t="inlineStr">
+        <is>
+          <t>-1.36%</t>
+        </is>
+      </c>
+      <c r="E2287" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2287" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2288">
+      <c r="A2288" t="inlineStr">
+        <is>
+          <t>기아</t>
+        </is>
+      </c>
+      <c r="B2288" t="inlineStr">
+        <is>
+          <t>16,898</t>
+        </is>
+      </c>
+      <c r="C2288" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+      <c r="D2288" t="inlineStr">
+        <is>
+          <t>+0.15%</t>
+        </is>
+      </c>
+      <c r="E2288" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2288" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2289">
+      <c r="A2289" t="inlineStr">
+        <is>
+          <t>KODEX 200</t>
+        </is>
+      </c>
+      <c r="B2289" t="inlineStr">
+        <is>
+          <t>23,725</t>
+        </is>
+      </c>
+      <c r="C2289" t="inlineStr">
+        <is>
+          <t>751</t>
+        </is>
+      </c>
+      <c r="D2289" t="inlineStr">
+        <is>
+          <t>-0.17%</t>
+        </is>
+      </c>
+      <c r="E2289" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2289" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2290">
+      <c r="A2290" t="inlineStr">
+        <is>
+          <t>현대차</t>
+        </is>
+      </c>
+      <c r="B2290" t="inlineStr">
+        <is>
+          <t>11,856</t>
+        </is>
+      </c>
+      <c r="C2290" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D2290" t="inlineStr">
+        <is>
+          <t>+1.47%</t>
+        </is>
+      </c>
+      <c r="E2290" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2290" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2291">
+      <c r="A2291" t="inlineStr">
+        <is>
+          <t>한화솔루션</t>
+        </is>
+      </c>
+      <c r="B2291" t="inlineStr">
+        <is>
+          <t>22,942</t>
+        </is>
+      </c>
+      <c r="C2291" t="inlineStr">
+        <is>
+          <t>471</t>
+        </is>
+      </c>
+      <c r="D2291" t="inlineStr">
+        <is>
+          <t>+2.94%</t>
+        </is>
+      </c>
+      <c r="E2291" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2291" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2292">
+      <c r="A2292" t="inlineStr">
+        <is>
+          <t>카카오뱅크</t>
+        </is>
+      </c>
+      <c r="B2292" t="inlineStr">
+        <is>
+          <t>8,122</t>
+        </is>
+      </c>
+      <c r="C2292" t="inlineStr">
+        <is>
+          <t>356</t>
+        </is>
+      </c>
+      <c r="D2292" t="inlineStr">
+        <is>
+          <t>-2.37%</t>
+        </is>
+      </c>
+      <c r="E2292" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2292" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2293">
+      <c r="A2293" t="inlineStr">
+        <is>
+          <t>TIGER 200TR</t>
+        </is>
+      </c>
+      <c r="B2293" t="inlineStr">
+        <is>
+          <t>22,336</t>
+        </is>
+      </c>
+      <c r="C2293" t="inlineStr">
+        <is>
+          <t>1,297</t>
+        </is>
+      </c>
+      <c r="D2293" t="inlineStr">
+        <is>
+          <t>-0.32%</t>
+        </is>
+      </c>
+      <c r="E2293" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2293" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2294">
+      <c r="A2294" t="inlineStr">
+        <is>
+          <t>현대미포조선</t>
+        </is>
+      </c>
+      <c r="B2294" t="inlineStr">
+        <is>
+          <t>7,606</t>
+        </is>
+      </c>
+      <c r="C2294" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="D2294" t="inlineStr">
+        <is>
+          <t>+0.44%</t>
+        </is>
+      </c>
+      <c r="E2294" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2294" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2295">
+      <c r="A2295" t="inlineStr">
+        <is>
+          <t>삼성전자우</t>
+        </is>
+      </c>
+      <c r="B2295" t="inlineStr">
+        <is>
+          <t>21,542</t>
+        </is>
+      </c>
+      <c r="C2295" t="inlineStr">
+        <is>
+          <t>383</t>
+        </is>
+      </c>
+      <c r="D2295" t="inlineStr">
+        <is>
+          <t>-0.88%</t>
+        </is>
+      </c>
+      <c r="E2295" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2295" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2296">
+      <c r="A2296" t="inlineStr">
+        <is>
+          <t>S-Oil</t>
+        </is>
+      </c>
+      <c r="B2296" t="inlineStr">
+        <is>
+          <t>5,709</t>
+        </is>
+      </c>
+      <c r="C2296" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="D2296" t="inlineStr">
+        <is>
+          <t>-2.39%</t>
+        </is>
+      </c>
+      <c r="E2296" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2296" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2297">
+      <c r="A2297" t="inlineStr">
+        <is>
+          <t>OCI</t>
+        </is>
+      </c>
+      <c r="B2297" t="inlineStr">
+        <is>
+          <t>21,414</t>
+        </is>
+      </c>
+      <c r="C2297" t="inlineStr">
+        <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="D2297" t="inlineStr">
+        <is>
+          <t>+0.98%</t>
+        </is>
+      </c>
+      <c r="E2297" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2297" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2298">
+      <c r="A2298" t="inlineStr">
+        <is>
+          <t>하나금융지주</t>
+        </is>
+      </c>
+      <c r="B2298" t="inlineStr">
+        <is>
+          <t>5,557</t>
+        </is>
+      </c>
+      <c r="C2298" t="inlineStr">
+        <is>
+          <t>136</t>
+        </is>
+      </c>
+      <c r="D2298" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2298" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2298" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2299">
+      <c r="A2299" t="inlineStr">
+        <is>
+          <t>LG화학</t>
+        </is>
+      </c>
+      <c r="B2299" t="inlineStr">
+        <is>
+          <t>19,259</t>
+        </is>
+      </c>
+      <c r="C2299" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="D2299" t="inlineStr">
+        <is>
+          <t>-0.56%</t>
+        </is>
+      </c>
+      <c r="E2299" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2299" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2300">
+      <c r="A2300" t="inlineStr">
+        <is>
+          <t>아모레퍼시픽</t>
+        </is>
+      </c>
+      <c r="B2300" t="inlineStr">
+        <is>
+          <t>5,268</t>
+        </is>
+      </c>
+      <c r="C2300" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D2300" t="inlineStr">
+        <is>
+          <t>-0.44%</t>
+        </is>
+      </c>
+      <c r="E2300" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2300" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2301">
+      <c r="A2301" t="inlineStr">
+        <is>
+          <t>삼성전자</t>
+        </is>
+      </c>
+      <c r="B2301" t="inlineStr">
+        <is>
+          <t>16,672</t>
+        </is>
+      </c>
+      <c r="C2301" t="inlineStr">
+        <is>
+          <t>268</t>
+        </is>
+      </c>
+      <c r="D2301" t="inlineStr">
+        <is>
+          <t>-1.13%</t>
+        </is>
+      </c>
+      <c r="E2301" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2301" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2302">
+      <c r="A2302" t="inlineStr">
+        <is>
+          <t>CJ대한통운</t>
+        </is>
+      </c>
+      <c r="B2302" t="inlineStr">
+        <is>
+          <t>4,422</t>
+        </is>
+      </c>
+      <c r="C2302" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="D2302" t="inlineStr">
+        <is>
+          <t>-1.04%</t>
+        </is>
+      </c>
+      <c r="E2302" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2302" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2303">
+      <c r="A2303" t="inlineStr">
+        <is>
+          <t>포스코케미칼</t>
+        </is>
+      </c>
+      <c r="B2303" t="inlineStr">
+        <is>
+          <t>16,400</t>
+        </is>
+      </c>
+      <c r="C2303" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="D2303" t="inlineStr">
+        <is>
+          <t>+2.08%</t>
+        </is>
+      </c>
+      <c r="E2303" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2303" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2304">
+      <c r="A2304" t="inlineStr">
+        <is>
+          <t>SK이노베이션</t>
+        </is>
+      </c>
+      <c r="B2304" t="inlineStr">
+        <is>
+          <t>3,668</t>
+        </is>
+      </c>
+      <c r="C2304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D2304" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2304" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2304" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2305">
+      <c r="A2305" t="inlineStr">
+        <is>
+          <t>KB금융</t>
+        </is>
+      </c>
+      <c r="B2305" t="inlineStr">
+        <is>
+          <t>13,165</t>
+        </is>
+      </c>
+      <c r="C2305" t="inlineStr">
+        <is>
+          <t>270</t>
+        </is>
+      </c>
+      <c r="D2305" t="inlineStr">
+        <is>
+          <t>+0.41%</t>
+        </is>
+      </c>
+      <c r="E2305" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2305" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2306">
+      <c r="A2306" t="inlineStr">
+        <is>
+          <t>KODEX WTI원유선물인버스(H)</t>
+        </is>
+      </c>
+      <c r="B2306" t="inlineStr">
+        <is>
+          <t>3,220</t>
+        </is>
+      </c>
+      <c r="C2306" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="D2306" t="inlineStr">
+        <is>
+          <t>+3.04%</t>
+        </is>
+      </c>
+      <c r="E2306" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2306" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2307">
+      <c r="A2307" t="inlineStr">
+        <is>
+          <t>삼성바이오로직스</t>
+        </is>
+      </c>
+      <c r="B2307" t="inlineStr">
+        <is>
+          <t>12,342</t>
+        </is>
+      </c>
+      <c r="C2307" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D2307" t="inlineStr">
+        <is>
+          <t>+1.01%</t>
+        </is>
+      </c>
+      <c r="E2307" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2307" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2308">
+      <c r="A2308" t="inlineStr">
+        <is>
+          <t>하이브</t>
+        </is>
+      </c>
+      <c r="B2308" t="inlineStr">
+        <is>
+          <t>3,136</t>
+        </is>
+      </c>
+      <c r="C2308" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D2308" t="inlineStr">
+        <is>
+          <t>-1.15%</t>
+        </is>
+      </c>
+      <c r="E2308" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2308" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2309">
+      <c r="A2309" t="inlineStr">
+        <is>
+          <t>LX세미콘</t>
+        </is>
+      </c>
+      <c r="B2309" t="inlineStr">
+        <is>
+          <t>11,964</t>
+        </is>
+      </c>
+      <c r="C2309" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="D2309" t="inlineStr">
+        <is>
+          <t>-2.09%</t>
+        </is>
+      </c>
+      <c r="E2309" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2309" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2310">
+      <c r="A2310" t="inlineStr">
+        <is>
+          <t>한미글로벌</t>
+        </is>
+      </c>
+      <c r="B2310" t="inlineStr">
+        <is>
+          <t>2,997</t>
+        </is>
+      </c>
+      <c r="C2310" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="D2310" t="inlineStr">
+        <is>
+          <t>+0.22%</t>
+        </is>
+      </c>
+      <c r="E2310" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2310" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2311">
+      <c r="A2311" t="inlineStr">
+        <is>
+          <t>KODEX 레버리지</t>
+        </is>
+      </c>
+      <c r="B2311" t="inlineStr">
+        <is>
+          <t>11,008</t>
+        </is>
+      </c>
+      <c r="C2311" t="inlineStr">
+        <is>
+          <t>754</t>
+        </is>
+      </c>
+      <c r="D2311" t="inlineStr">
+        <is>
+          <t>-0.44%</t>
+        </is>
+      </c>
+      <c r="E2311" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2311" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2312">
+      <c r="A2312" t="inlineStr">
+        <is>
+          <t>TIGER 미국나스닥100</t>
+        </is>
+      </c>
+      <c r="B2312" t="inlineStr">
+        <is>
+          <t>2,854</t>
+        </is>
+      </c>
+      <c r="C2312" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="D2312" t="inlineStr">
+        <is>
+          <t>-1.98%</t>
+        </is>
+      </c>
+      <c r="E2312" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2312" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2313">
+      <c r="A2313" t="inlineStr">
+        <is>
+          <t>신한지주</t>
+        </is>
+      </c>
+      <c r="B2313" t="inlineStr">
+        <is>
+          <t>10,127</t>
+        </is>
+      </c>
+      <c r="C2313" t="inlineStr">
+        <is>
+          <t>272</t>
+        </is>
+      </c>
+      <c r="D2313" t="inlineStr">
+        <is>
+          <t>-0.13%</t>
+        </is>
+      </c>
+      <c r="E2313" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2313" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2314">
+      <c r="A2314" t="inlineStr">
+        <is>
+          <t>LG생활건강</t>
+        </is>
+      </c>
+      <c r="B2314" t="inlineStr">
+        <is>
+          <t>2,459</t>
+        </is>
+      </c>
+      <c r="C2314" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D2314" t="inlineStr">
+        <is>
+          <t>+0.52%</t>
+        </is>
+      </c>
+      <c r="E2314" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2314" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2315">
+      <c r="A2315" t="inlineStr">
+        <is>
+          <t>TIGER 200</t>
+        </is>
+      </c>
+      <c r="B2315" t="inlineStr">
+        <is>
+          <t>8,743</t>
+        </is>
+      </c>
+      <c r="C2315" t="inlineStr">
+        <is>
+          <t>277</t>
+        </is>
+      </c>
+      <c r="D2315" t="inlineStr">
+        <is>
+          <t>-0.17%</t>
+        </is>
+      </c>
+      <c r="E2315" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2315" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2316">
+      <c r="A2316" t="inlineStr">
+        <is>
+          <t>KODEX 코스닥150</t>
+        </is>
+      </c>
+      <c r="B2316" t="inlineStr">
+        <is>
+          <t>2,440</t>
+        </is>
+      </c>
+      <c r="C2316" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="D2316" t="inlineStr">
+        <is>
+          <t>-0.59%</t>
+        </is>
+      </c>
+      <c r="E2316" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2316" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2317">
+      <c r="A2317" t="inlineStr">
+        <is>
+          <t>두산에너빌리티</t>
+        </is>
+      </c>
+      <c r="B2317" t="inlineStr">
+        <is>
+          <t>8,105</t>
+        </is>
+      </c>
+      <c r="C2317" t="inlineStr">
+        <is>
+          <t>508</t>
+        </is>
+      </c>
+      <c r="D2317" t="inlineStr">
+        <is>
+          <t>+0.31%</t>
+        </is>
+      </c>
+      <c r="E2317" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2317" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2318">
+      <c r="A2318" t="inlineStr">
+        <is>
+          <t>LG디스플레이</t>
+        </is>
+      </c>
+      <c r="B2318" t="inlineStr">
+        <is>
+          <t>2,394</t>
+        </is>
+      </c>
+      <c r="C2318" t="inlineStr">
+        <is>
+          <t>166</t>
+        </is>
+      </c>
+      <c r="D2318" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2318" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2318" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2319">
+      <c r="A2319" t="inlineStr">
+        <is>
+          <t>씨에스윈드</t>
+        </is>
+      </c>
+      <c r="B2319" t="inlineStr">
+        <is>
+          <t>8,070</t>
+        </is>
+      </c>
+      <c r="C2319" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="D2319" t="inlineStr">
+        <is>
+          <t>+3.79%</t>
+        </is>
+      </c>
+      <c r="E2319" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2319" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2320">
+      <c r="A2320" t="inlineStr">
+        <is>
+          <t>해성디에스</t>
+        </is>
+      </c>
+      <c r="B2320" t="inlineStr">
+        <is>
+          <t>2,353</t>
+        </is>
+      </c>
+      <c r="C2320" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="D2320" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2320" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2320" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2321">
+      <c r="A2321" t="inlineStr">
+        <is>
+          <t>LG전자</t>
+        </is>
+      </c>
+      <c r="B2321" t="inlineStr">
+        <is>
+          <t>8,006</t>
+        </is>
+      </c>
+      <c r="C2321" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="D2321" t="inlineStr">
+        <is>
+          <t>-0.64%</t>
+        </is>
+      </c>
+      <c r="E2321" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2321" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2322">
+      <c r="A2322" t="inlineStr">
+        <is>
+          <t>TIGER 미국테크TOP10 INDXX</t>
+        </is>
+      </c>
+      <c r="B2322" t="inlineStr">
+        <is>
+          <t>2,276</t>
+        </is>
+      </c>
+      <c r="C2322" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="D2322" t="inlineStr">
+        <is>
+          <t>-2.86%</t>
+        </is>
+      </c>
+      <c r="E2322" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2322" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2323">
+      <c r="A2323" t="inlineStr">
+        <is>
+          <t>현대두산인프라코어</t>
+        </is>
+      </c>
+      <c r="B2323" t="inlineStr">
+        <is>
+          <t>7,702</t>
+        </is>
+      </c>
+      <c r="C2323" t="inlineStr">
+        <is>
+          <t>1,071</t>
+        </is>
+      </c>
+      <c r="D2323" t="inlineStr">
+        <is>
+          <t>-0.82%</t>
+        </is>
+      </c>
+      <c r="E2323" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2323" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2324">
+      <c r="A2324" t="inlineStr">
+        <is>
+          <t>자화전자</t>
+        </is>
+      </c>
+      <c r="B2324" t="inlineStr">
+        <is>
+          <t>2,251</t>
+        </is>
+      </c>
+      <c r="C2324" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="D2324" t="inlineStr">
+        <is>
+          <t>-0.25%</t>
+        </is>
+      </c>
+      <c r="E2324" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2324" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2325">
+      <c r="A2325" t="inlineStr">
+        <is>
+          <t>LG이노텍</t>
+        </is>
+      </c>
+      <c r="B2325" t="inlineStr">
+        <is>
+          <t>7,268</t>
+        </is>
+      </c>
+      <c r="C2325" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D2325" t="inlineStr">
+        <is>
+          <t>-0.86%</t>
+        </is>
+      </c>
+      <c r="E2325" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2325" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2326">
+      <c r="A2326" t="inlineStr">
+        <is>
+          <t>셀트리온</t>
+        </is>
+      </c>
+      <c r="B2326" t="inlineStr">
+        <is>
+          <t>2,188</t>
+        </is>
+      </c>
+      <c r="C2326" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D2326" t="inlineStr">
+        <is>
+          <t>+1.33%</t>
+        </is>
+      </c>
+      <c r="E2326" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2326" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2327">
+      <c r="A2327" t="inlineStr">
+        <is>
+          <t>이수화학</t>
+        </is>
+      </c>
+      <c r="B2327" t="inlineStr">
+        <is>
+          <t>6,924</t>
+        </is>
+      </c>
+      <c r="C2327" t="inlineStr">
+        <is>
+          <t>236</t>
+        </is>
+      </c>
+      <c r="D2327" t="inlineStr">
+        <is>
+          <t>+2.21%</t>
+        </is>
+      </c>
+      <c r="E2327" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2327" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2328">
+      <c r="A2328" t="inlineStr">
+        <is>
+          <t>KODEX 코스닥150레버리지</t>
+        </is>
+      </c>
+      <c r="B2328" t="inlineStr">
+        <is>
+          <t>2,123</t>
+        </is>
+      </c>
+      <c r="C2328" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="D2328" t="inlineStr">
+        <is>
+          <t>-1.52%</t>
+        </is>
+      </c>
+      <c r="E2328" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2328" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2329">
+      <c r="A2329" t="inlineStr">
+        <is>
+          <t>삼성물산</t>
+        </is>
+      </c>
+      <c r="B2329" t="inlineStr">
+        <is>
+          <t>6,673</t>
+        </is>
+      </c>
+      <c r="C2329" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D2329" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2329" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2329" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2330">
+      <c r="A2330" t="inlineStr">
+        <is>
+          <t>DGB금융지주</t>
+        </is>
+      </c>
+      <c r="B2330" t="inlineStr">
+        <is>
+          <t>2,107</t>
+        </is>
+      </c>
+      <c r="C2330" t="inlineStr">
+        <is>
+          <t>309</t>
+        </is>
+      </c>
+      <c r="D2330" t="inlineStr">
+        <is>
+          <t>-0.29%</t>
+        </is>
+      </c>
+      <c r="E2330" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2330" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2331">
+      <c r="A2331" t="inlineStr">
+        <is>
+          <t>한국전력</t>
+        </is>
+      </c>
+      <c r="B2331" t="inlineStr">
+        <is>
+          <t>5,920</t>
+        </is>
+      </c>
+      <c r="C2331" t="inlineStr">
+        <is>
+          <t>330</t>
+        </is>
+      </c>
+      <c r="D2331" t="inlineStr">
+        <is>
+          <t>-2.42%</t>
+        </is>
+      </c>
+      <c r="E2331" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2331" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2332">
+      <c r="A2332" t="inlineStr">
+        <is>
+          <t>에이프로젠</t>
+        </is>
+      </c>
+      <c r="B2332" t="inlineStr">
+        <is>
+          <t>1,738</t>
+        </is>
+      </c>
+      <c r="C2332" t="inlineStr">
+        <is>
+          <t>1,657</t>
+        </is>
+      </c>
+      <c r="D2332" t="inlineStr">
+        <is>
+          <t>+0.49%</t>
+        </is>
+      </c>
+      <c r="E2332" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2332" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2333">
+      <c r="A2333" t="inlineStr">
+        <is>
+          <t>GS리테일</t>
+        </is>
+      </c>
+      <c r="B2333" t="inlineStr">
+        <is>
+          <t>5,919</t>
+        </is>
+      </c>
+      <c r="C2333" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+      <c r="D2333" t="inlineStr">
+        <is>
+          <t>+0.17%</t>
+        </is>
+      </c>
+      <c r="E2333" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2333" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2334">
+      <c r="A2334" t="inlineStr">
+        <is>
+          <t>영풍</t>
+        </is>
+      </c>
+      <c r="B2334" t="inlineStr">
+        <is>
+          <t>1,584</t>
+        </is>
+      </c>
+      <c r="C2334" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2334" t="inlineStr">
+        <is>
+          <t>-3.63%</t>
+        </is>
+      </c>
+      <c r="E2334" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2334" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2335">
+      <c r="A2335" t="inlineStr">
+        <is>
+          <t>LIG넥스원</t>
+        </is>
+      </c>
+      <c r="B2335" t="inlineStr">
+        <is>
+          <t>5,571</t>
+        </is>
+      </c>
+      <c r="C2335" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="D2335" t="inlineStr">
+        <is>
+          <t>+0.10%</t>
+        </is>
+      </c>
+      <c r="E2335" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2335" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2336">
+      <c r="A2336" t="inlineStr">
+        <is>
+          <t>더블유게임즈</t>
+        </is>
+      </c>
+      <c r="B2336" t="inlineStr">
+        <is>
+          <t>1,507</t>
+        </is>
+      </c>
+      <c r="C2336" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="D2336" t="inlineStr">
+        <is>
+          <t>+0.43%</t>
+        </is>
+      </c>
+      <c r="E2336" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2336" t="inlineStr">
+        <is>
+          <t>2022-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2337">
+      <c r="A2337" t="inlineStr">
+        <is>
+          <t>SK하이닉스</t>
+        </is>
+      </c>
+      <c r="B2337" t="inlineStr">
+        <is>
+          <t>49,867</t>
+        </is>
+      </c>
+      <c r="C2337" t="inlineStr">
+        <is>
+          <t>557</t>
+        </is>
+      </c>
+      <c r="D2337" t="inlineStr">
+        <is>
+          <t>+5.27%</t>
+        </is>
+      </c>
+      <c r="E2337" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2337" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2338">
+      <c r="A2338" t="inlineStr">
+        <is>
+          <t>삼성전자</t>
+        </is>
+      </c>
+      <c r="B2338" t="inlineStr">
+        <is>
+          <t>242,733</t>
+        </is>
+      </c>
+      <c r="C2338" t="inlineStr">
+        <is>
+          <t>3,990</t>
+        </is>
+      </c>
+      <c r="D2338" t="inlineStr">
+        <is>
+          <t>+3.97%</t>
+        </is>
+      </c>
+      <c r="E2338" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2338" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2339">
+      <c r="A2339" t="inlineStr">
+        <is>
+          <t>LG에너지솔루션</t>
+        </is>
+      </c>
+      <c r="B2339" t="inlineStr">
+        <is>
+          <t>31,861</t>
+        </is>
+      </c>
+      <c r="C2339" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D2339" t="inlineStr">
+        <is>
+          <t>+3.80%</t>
+        </is>
+      </c>
+      <c r="E2339" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2339" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2340">
+      <c r="A2340" t="inlineStr">
+        <is>
+          <t>POSCO홀딩스</t>
+        </is>
+      </c>
+      <c r="B2340" t="inlineStr">
+        <is>
+          <t>58,425</t>
+        </is>
+      </c>
+      <c r="C2340" t="inlineStr">
+        <is>
+          <t>206</t>
+        </is>
+      </c>
+      <c r="D2340" t="inlineStr">
+        <is>
+          <t>+0.89%</t>
+        </is>
+      </c>
+      <c r="E2340" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2340" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2341">
+      <c r="A2341" t="inlineStr">
+        <is>
+          <t>삼성바이오로직스</t>
+        </is>
+      </c>
+      <c r="B2341" t="inlineStr">
+        <is>
+          <t>30,696</t>
+        </is>
+      </c>
+      <c r="C2341" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D2341" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2341" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2341" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2342">
+      <c r="A2342" t="inlineStr">
+        <is>
+          <t>NAVER</t>
+        </is>
+      </c>
+      <c r="B2342" t="inlineStr">
+        <is>
+          <t>44,304</t>
+        </is>
+      </c>
+      <c r="C2342" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="D2342" t="inlineStr">
+        <is>
+          <t>+8.81%</t>
+        </is>
+      </c>
+      <c r="E2342" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2342" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2343">
+      <c r="A2343" t="inlineStr">
+        <is>
+          <t>현대차</t>
+        </is>
+      </c>
+      <c r="B2343" t="inlineStr">
+        <is>
+          <t>26,474</t>
+        </is>
+      </c>
+      <c r="C2343" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
+      </c>
+      <c r="D2343" t="inlineStr">
+        <is>
+          <t>+2.06%</t>
+        </is>
+      </c>
+      <c r="E2343" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2343" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2344">
+      <c r="A2344" t="inlineStr">
+        <is>
+          <t>금양</t>
+        </is>
+      </c>
+      <c r="B2344" t="inlineStr">
+        <is>
+          <t>24,010</t>
+        </is>
+      </c>
+      <c r="C2344" t="inlineStr">
+        <is>
+          <t>664</t>
+        </is>
+      </c>
+      <c r="D2344" t="inlineStr">
+        <is>
+          <t>-6.89%</t>
+        </is>
+      </c>
+      <c r="E2344" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2344" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2345">
+      <c r="A2345" t="inlineStr">
+        <is>
+          <t>KODEX 200</t>
+        </is>
+      </c>
+      <c r="B2345" t="inlineStr">
+        <is>
+          <t>24,897</t>
+        </is>
+      </c>
+      <c r="C2345" t="inlineStr">
+        <is>
+          <t>801</t>
+        </is>
+      </c>
+      <c r="D2345" t="inlineStr">
+        <is>
+          <t>+3.52%</t>
+        </is>
+      </c>
+      <c r="E2345" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2345" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2346">
+      <c r="A2346" t="inlineStr">
+        <is>
+          <t>LG화학</t>
+        </is>
+      </c>
+      <c r="B2346" t="inlineStr">
+        <is>
+          <t>13,034</t>
+        </is>
+      </c>
+      <c r="C2346" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D2346" t="inlineStr">
+        <is>
+          <t>+5.61%</t>
+        </is>
+      </c>
+      <c r="E2346" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2346" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2347">
+      <c r="A2347" t="inlineStr">
+        <is>
+          <t>TIGER 200</t>
+        </is>
+      </c>
+      <c r="B2347" t="inlineStr">
+        <is>
+          <t>22,119</t>
+        </is>
+      </c>
+      <c r="C2347" t="inlineStr">
+        <is>
+          <t>710</t>
+        </is>
+      </c>
+      <c r="D2347" t="inlineStr">
+        <is>
+          <t>+3.45%</t>
+        </is>
+      </c>
+      <c r="E2347" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2347" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2348">
+      <c r="A2348" t="inlineStr">
+        <is>
+          <t>포스코케미칼</t>
+        </is>
+      </c>
+      <c r="B2348" t="inlineStr">
+        <is>
+          <t>10,943</t>
+        </is>
+      </c>
+      <c r="C2348" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="D2348" t="inlineStr">
+        <is>
+          <t>+2.05%</t>
+        </is>
+      </c>
+      <c r="E2348" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2348" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2349">
+      <c r="A2349" t="inlineStr">
+        <is>
+          <t>삼성전자우</t>
+        </is>
+      </c>
+      <c r="B2349" t="inlineStr">
+        <is>
+          <t>14,315</t>
+        </is>
+      </c>
+      <c r="C2349" t="inlineStr">
+        <is>
+          <t>257</t>
+        </is>
+      </c>
+      <c r="D2349" t="inlineStr">
+        <is>
+          <t>+3.42%</t>
+        </is>
+      </c>
+      <c r="E2349" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2349" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2350">
+      <c r="A2350" t="inlineStr">
+        <is>
+          <t>삼성SDI</t>
+        </is>
+      </c>
+      <c r="B2350" t="inlineStr">
+        <is>
+          <t>10,844</t>
+        </is>
+      </c>
+      <c r="C2350" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D2350" t="inlineStr">
+        <is>
+          <t>+1.93%</t>
+        </is>
+      </c>
+      <c r="E2350" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2350" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2351">
+      <c r="A2351" t="inlineStr">
+        <is>
+          <t>LG이노텍</t>
+        </is>
+      </c>
+      <c r="B2351" t="inlineStr">
+        <is>
+          <t>13,489</t>
+        </is>
+      </c>
+      <c r="C2351" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D2351" t="inlineStr">
+        <is>
+          <t>+7.48%</t>
+        </is>
+      </c>
+      <c r="E2351" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2351" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2352">
+      <c r="A2352" t="inlineStr">
+        <is>
+          <t>두산에너빌리티</t>
+        </is>
+      </c>
+      <c r="B2352" t="inlineStr">
+        <is>
+          <t>10,265</t>
+        </is>
+      </c>
+      <c r="C2352" t="inlineStr">
+        <is>
+          <t>633</t>
+        </is>
+      </c>
+      <c r="D2352" t="inlineStr">
+        <is>
+          <t>+2.21%</t>
+        </is>
+      </c>
+      <c r="E2352" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2352" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2353">
+      <c r="A2353" t="inlineStr">
+        <is>
+          <t>오리온</t>
+        </is>
+      </c>
+      <c r="B2353" t="inlineStr">
+        <is>
+          <t>11,939</t>
+        </is>
+      </c>
+      <c r="C2353" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
+      </c>
+      <c r="D2353" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2353" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2353" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2354">
+      <c r="A2354" t="inlineStr">
+        <is>
+          <t>기아</t>
+        </is>
+      </c>
+      <c r="B2354" t="inlineStr">
+        <is>
+          <t>9,393</t>
+        </is>
+      </c>
+      <c r="C2354" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="D2354" t="inlineStr">
+        <is>
+          <t>+1.95%</t>
+        </is>
+      </c>
+      <c r="E2354" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2354" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2355">
+      <c r="A2355" t="inlineStr">
+        <is>
+          <t>DN오토모티브</t>
+        </is>
+      </c>
+      <c r="B2355" t="inlineStr">
+        <is>
+          <t>10,916</t>
+        </is>
+      </c>
+      <c r="C2355" t="inlineStr">
+        <is>
+          <t>177</t>
+        </is>
+      </c>
+      <c r="D2355" t="inlineStr">
+        <is>
+          <t>-1.31%</t>
+        </is>
+      </c>
+      <c r="E2355" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2355" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2356">
+      <c r="A2356" t="inlineStr">
+        <is>
+          <t>카카오페이</t>
+        </is>
+      </c>
+      <c r="B2356" t="inlineStr">
+        <is>
+          <t>8,383</t>
+        </is>
+      </c>
+      <c r="C2356" t="inlineStr">
+        <is>
+          <t>183</t>
+        </is>
+      </c>
+      <c r="D2356" t="inlineStr">
+        <is>
+          <t>+17.52%</t>
+        </is>
+      </c>
+      <c r="E2356" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2356" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2357">
+      <c r="A2357" t="inlineStr">
+        <is>
+          <t>LG전자</t>
+        </is>
+      </c>
+      <c r="B2357" t="inlineStr">
+        <is>
+          <t>9,698</t>
+        </is>
+      </c>
+      <c r="C2357" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="D2357" t="inlineStr">
+        <is>
+          <t>+2.83%</t>
+        </is>
+      </c>
+      <c r="E2357" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2357" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2358">
+      <c r="A2358" t="inlineStr">
+        <is>
+          <t>카카오뱅크</t>
+        </is>
+      </c>
+      <c r="B2358" t="inlineStr">
+        <is>
+          <t>7,612</t>
+        </is>
+      </c>
+      <c r="C2358" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="D2358" t="inlineStr">
+        <is>
+          <t>+13.73%</t>
+        </is>
+      </c>
+      <c r="E2358" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2358" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2359">
+      <c r="A2359" t="inlineStr">
+        <is>
+          <t>우리금융지주</t>
+        </is>
+      </c>
+      <c r="B2359" t="inlineStr">
+        <is>
+          <t>7,233</t>
+        </is>
+      </c>
+      <c r="C2359" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="D2359" t="inlineStr">
+        <is>
+          <t>+0.85%</t>
+        </is>
+      </c>
+      <c r="E2359" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2359" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2360">
+      <c r="A2360" t="inlineStr">
+        <is>
+          <t>이수화학</t>
+        </is>
+      </c>
+      <c r="B2360" t="inlineStr">
+        <is>
+          <t>6,944</t>
+        </is>
+      </c>
+      <c r="C2360" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
+      <c r="D2360" t="inlineStr">
+        <is>
+          <t>+3.45%</t>
+        </is>
+      </c>
+      <c r="E2360" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2360" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2361">
+      <c r="A2361" t="inlineStr">
+        <is>
+          <t>삼성물산</t>
+        </is>
+      </c>
+      <c r="B2361" t="inlineStr">
+        <is>
+          <t>7,215</t>
+        </is>
+      </c>
+      <c r="C2361" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="D2361" t="inlineStr">
+        <is>
+          <t>+1.65%</t>
+        </is>
+      </c>
+      <c r="E2361" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2361" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2362">
+      <c r="A2362" t="inlineStr">
+        <is>
+          <t>KODEX 인버스</t>
+        </is>
+      </c>
+      <c r="B2362" t="inlineStr">
+        <is>
+          <t>5,889</t>
+        </is>
+      </c>
+      <c r="C2362" t="inlineStr">
+        <is>
+          <t>1,202</t>
+        </is>
+      </c>
+      <c r="D2362" t="inlineStr">
+        <is>
+          <t>-3.36%</t>
+        </is>
+      </c>
+      <c r="E2362" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2362" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2363">
+      <c r="A2363" t="inlineStr">
+        <is>
+          <t>KODEX 200선물인버스2X</t>
+        </is>
+      </c>
+      <c r="B2363" t="inlineStr">
+        <is>
+          <t>7,113</t>
+        </is>
+      </c>
+      <c r="C2363" t="inlineStr">
+        <is>
+          <t>2,284</t>
+        </is>
+      </c>
+      <c r="D2363" t="inlineStr">
+        <is>
+          <t>-6.73%</t>
+        </is>
+      </c>
+      <c r="E2363" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2363" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2364">
+      <c r="A2364" t="inlineStr">
+        <is>
+          <t>일동제약</t>
+        </is>
+      </c>
+      <c r="B2364" t="inlineStr">
+        <is>
+          <t>5,860</t>
+        </is>
+      </c>
+      <c r="C2364" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D2364" t="inlineStr">
+        <is>
+          <t>+1.38%</t>
+        </is>
+      </c>
+      <c r="E2364" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2364" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2365">
+      <c r="A2365" t="inlineStr">
+        <is>
+          <t>OCI</t>
+        </is>
+      </c>
+      <c r="B2365" t="inlineStr">
+        <is>
+          <t>6,884</t>
+        </is>
+      </c>
+      <c r="C2365" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="D2365" t="inlineStr">
+        <is>
+          <t>+2.97%</t>
+        </is>
+      </c>
+      <c r="E2365" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2365" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2366">
+      <c r="A2366" t="inlineStr">
+        <is>
+          <t>현대로템</t>
+        </is>
+      </c>
+      <c r="B2366" t="inlineStr">
+        <is>
+          <t>5,508</t>
+        </is>
+      </c>
+      <c r="C2366" t="inlineStr">
+        <is>
+          <t>206</t>
+        </is>
+      </c>
+      <c r="D2366" t="inlineStr">
+        <is>
+          <t>+1.37%</t>
+        </is>
+      </c>
+      <c r="E2366" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2366" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2367">
+      <c r="A2367" t="inlineStr">
+        <is>
+          <t>HL만도</t>
+        </is>
+      </c>
+      <c r="B2367" t="inlineStr">
+        <is>
+          <t>6,715</t>
+        </is>
+      </c>
+      <c r="C2367" t="inlineStr">
+        <is>
+          <t>132</t>
+        </is>
+      </c>
+      <c r="D2367" t="inlineStr">
+        <is>
+          <t>+0.98%</t>
+        </is>
+      </c>
+      <c r="E2367" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2367" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2368">
+      <c r="A2368" t="inlineStr">
+        <is>
+          <t>KT</t>
+        </is>
+      </c>
+      <c r="B2368" t="inlineStr">
+        <is>
+          <t>5,094</t>
+        </is>
+      </c>
+      <c r="C2368" t="inlineStr">
+        <is>
+          <t>138</t>
+        </is>
+      </c>
+      <c r="D2368" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2368" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2368" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2369">
+      <c r="A2369" t="inlineStr">
+        <is>
+          <t>삼성전기</t>
+        </is>
+      </c>
+      <c r="B2369" t="inlineStr">
+        <is>
+          <t>6,466</t>
+        </is>
+      </c>
+      <c r="C2369" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D2369" t="inlineStr">
+        <is>
+          <t>+4.40%</t>
+        </is>
+      </c>
+      <c r="E2369" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2369" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2370">
+      <c r="A2370" t="inlineStr">
+        <is>
+          <t>신세계</t>
+        </is>
+      </c>
+      <c r="B2370" t="inlineStr">
+        <is>
+          <t>4,517</t>
+        </is>
+      </c>
+      <c r="C2370" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D2370" t="inlineStr">
+        <is>
+          <t>+1.20%</t>
+        </is>
+      </c>
+      <c r="E2370" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2370" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2371">
+      <c r="A2371" t="inlineStr">
+        <is>
+          <t>삼성엔지니어링</t>
+        </is>
+      </c>
+      <c r="B2371" t="inlineStr">
+        <is>
+          <t>6,442</t>
+        </is>
+      </c>
+      <c r="C2371" t="inlineStr">
+        <is>
+          <t>252</t>
+        </is>
+      </c>
+      <c r="D2371" t="inlineStr">
+        <is>
+          <t>+2.54%</t>
+        </is>
+      </c>
+      <c r="E2371" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2371" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2372">
+      <c r="A2372" t="inlineStr">
+        <is>
+          <t>HMM</t>
+        </is>
+      </c>
+      <c r="B2372" t="inlineStr">
+        <is>
+          <t>4,232</t>
+        </is>
+      </c>
+      <c r="C2372" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
+      </c>
+      <c r="D2372" t="inlineStr">
+        <is>
+          <t>+3.21%</t>
+        </is>
+      </c>
+      <c r="E2372" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2372" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2373">
+      <c r="A2373" t="inlineStr">
+        <is>
+          <t>SK바이오사이언스</t>
+        </is>
+      </c>
+      <c r="B2373" t="inlineStr">
+        <is>
+          <t>5,997</t>
+        </is>
+      </c>
+      <c r="C2373" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="D2373" t="inlineStr">
+        <is>
+          <t>+5.55%</t>
+        </is>
+      </c>
+      <c r="E2373" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2373" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2374">
+      <c r="A2374" t="inlineStr">
+        <is>
+          <t>현대모비스</t>
+        </is>
+      </c>
+      <c r="B2374" t="inlineStr">
+        <is>
+          <t>3,876</t>
+        </is>
+      </c>
+      <c r="C2374" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D2374" t="inlineStr">
+        <is>
+          <t>+0.68%</t>
+        </is>
+      </c>
+      <c r="E2374" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2374" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2375">
+      <c r="A2375" t="inlineStr">
+        <is>
+          <t>삼성생명</t>
+        </is>
+      </c>
+      <c r="B2375" t="inlineStr">
+        <is>
+          <t>5,268</t>
+        </is>
+      </c>
+      <c r="C2375" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D2375" t="inlineStr">
+        <is>
+          <t>-0.74%</t>
+        </is>
+      </c>
+      <c r="E2375" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2375" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2376">
+      <c r="A2376" t="inlineStr">
+        <is>
+          <t>TIGER 미국S&amp;P500</t>
+        </is>
+      </c>
+      <c r="B2376" t="inlineStr">
+        <is>
+          <t>3,527</t>
+        </is>
+      </c>
+      <c r="C2376" t="inlineStr">
+        <is>
+          <t>275</t>
+        </is>
+      </c>
+      <c r="D2376" t="inlineStr">
+        <is>
+          <t>+3.05%</t>
+        </is>
+      </c>
+      <c r="E2376" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2376" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2377">
+      <c r="A2377" t="inlineStr">
+        <is>
+          <t>SK이노베이션</t>
+        </is>
+      </c>
+      <c r="B2377" t="inlineStr">
+        <is>
+          <t>5,153</t>
+        </is>
+      </c>
+      <c r="C2377" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="D2377" t="inlineStr">
+        <is>
+          <t>+0.83%</t>
+        </is>
+      </c>
+      <c r="E2377" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2377" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2378">
+      <c r="A2378" t="inlineStr">
+        <is>
+          <t>TIGER 미국나스닥100</t>
+        </is>
+      </c>
+      <c r="B2378" t="inlineStr">
+        <is>
+          <t>3,321</t>
+        </is>
+      </c>
+      <c r="C2378" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="D2378" t="inlineStr">
+        <is>
+          <t>+4.69%</t>
+        </is>
+      </c>
+      <c r="E2378" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2378" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2379">
+      <c r="A2379" t="inlineStr">
+        <is>
+          <t>현대미포조선</t>
+        </is>
+      </c>
+      <c r="B2379" t="inlineStr">
+        <is>
+          <t>4,840</t>
+        </is>
+      </c>
+      <c r="C2379" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="D2379" t="inlineStr">
+        <is>
+          <t>+5.52%</t>
+        </is>
+      </c>
+      <c r="E2379" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2379" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2380">
+      <c r="A2380" t="inlineStr">
+        <is>
+          <t>대덕전자</t>
+        </is>
+      </c>
+      <c r="B2380" t="inlineStr">
+        <is>
+          <t>3,267</t>
+        </is>
+      </c>
+      <c r="C2380" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
+      </c>
+      <c r="D2380" t="inlineStr">
+        <is>
+          <t>+5.10%</t>
+        </is>
+      </c>
+      <c r="E2380" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2380" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2381">
+      <c r="A2381" t="inlineStr">
+        <is>
+          <t>신한지주</t>
+        </is>
+      </c>
+      <c r="B2381" t="inlineStr">
+        <is>
+          <t>4,840</t>
+        </is>
+      </c>
+      <c r="C2381" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="D2381" t="inlineStr">
+        <is>
+          <t>+0.13%</t>
+        </is>
+      </c>
+      <c r="E2381" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2381" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2382">
+      <c r="A2382" t="inlineStr">
+        <is>
+          <t>TIGER 미국테크TOP10 INDXX</t>
+        </is>
+      </c>
+      <c r="B2382" t="inlineStr">
+        <is>
+          <t>3,246</t>
+        </is>
+      </c>
+      <c r="C2382" t="inlineStr">
+        <is>
+          <t>366</t>
+        </is>
+      </c>
+      <c r="D2382" t="inlineStr">
+        <is>
+          <t>+5.65%</t>
+        </is>
+      </c>
+      <c r="E2382" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2382" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2383">
+      <c r="A2383" t="inlineStr">
+        <is>
+          <t>한국항공우주</t>
+        </is>
+      </c>
+      <c r="B2383" t="inlineStr">
+        <is>
+          <t>4,803</t>
+        </is>
+      </c>
+      <c r="C2383" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="D2383" t="inlineStr">
+        <is>
+          <t>+1.38%</t>
+        </is>
+      </c>
+      <c r="E2383" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2383" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2384">
+      <c r="A2384" t="inlineStr">
+        <is>
+          <t>코스모신소재</t>
+        </is>
+      </c>
+      <c r="B2384" t="inlineStr">
+        <is>
+          <t>2,982</t>
+        </is>
+      </c>
+      <c r="C2384" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D2384" t="inlineStr">
+        <is>
+          <t>+1.68%</t>
+        </is>
+      </c>
+      <c r="E2384" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2384" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2385">
+      <c r="A2385" t="inlineStr">
+        <is>
+          <t>KODEX 레버리지</t>
+        </is>
+      </c>
+      <c r="B2385" t="inlineStr">
+        <is>
+          <t>4,579</t>
+        </is>
+      </c>
+      <c r="C2385" t="inlineStr">
+        <is>
+          <t>312</t>
+        </is>
+      </c>
+      <c r="D2385" t="inlineStr">
+        <is>
+          <t>+6.70%</t>
+        </is>
+      </c>
+      <c r="E2385" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2385" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2386">
+      <c r="A2386" t="inlineStr">
+        <is>
+          <t>LX세미콘</t>
+        </is>
+      </c>
+      <c r="B2386" t="inlineStr">
+        <is>
+          <t>2,917</t>
+        </is>
+      </c>
+      <c r="C2386" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D2386" t="inlineStr">
+        <is>
+          <t>+6.35%</t>
+        </is>
+      </c>
+      <c r="E2386" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2386" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2387">
+      <c r="A2387" t="inlineStr">
+        <is>
+          <t>LG</t>
+        </is>
+      </c>
+      <c r="B2387" t="inlineStr">
+        <is>
+          <t>4,521</t>
+        </is>
+      </c>
+      <c r="C2387" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D2387" t="inlineStr">
+        <is>
+          <t>+1.58%</t>
+        </is>
+      </c>
+      <c r="E2387" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2387" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2388">
+      <c r="A2388" t="inlineStr">
+        <is>
+          <t>서울가스</t>
+        </is>
+      </c>
+      <c r="B2388" t="inlineStr">
+        <is>
+          <t>2,703</t>
+        </is>
+      </c>
+      <c r="C2388" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D2388" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E2388" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2388" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2389">
+      <c r="A2389" t="inlineStr">
+        <is>
+          <t>현대두산인프라코어</t>
+        </is>
+      </c>
+      <c r="B2389" t="inlineStr">
+        <is>
+          <t>4,203</t>
+        </is>
+      </c>
+      <c r="C2389" t="inlineStr">
+        <is>
+          <t>594</t>
+        </is>
+      </c>
+      <c r="D2389" t="inlineStr">
+        <is>
+          <t>-0.14%</t>
+        </is>
+      </c>
+      <c r="E2389" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2389" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2390">
+      <c r="A2390" t="inlineStr">
+        <is>
+          <t>SK텔레콤</t>
+        </is>
+      </c>
+      <c r="B2390" t="inlineStr">
+        <is>
+          <t>2,537</t>
+        </is>
+      </c>
+      <c r="C2390" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="D2390" t="inlineStr">
+        <is>
+          <t>+0.79%</t>
+        </is>
+      </c>
+      <c r="E2390" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2390" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2391">
+      <c r="A2391" t="inlineStr">
+        <is>
+          <t>농심</t>
+        </is>
+      </c>
+      <c r="B2391" t="inlineStr">
+        <is>
+          <t>4,158</t>
+        </is>
+      </c>
+      <c r="C2391" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D2391" t="inlineStr">
+        <is>
+          <t>-0.81%</t>
+        </is>
+      </c>
+      <c r="E2391" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2391" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2392">
+      <c r="A2392" t="inlineStr">
+        <is>
+          <t>호텔신라</t>
+        </is>
+      </c>
+      <c r="B2392" t="inlineStr">
+        <is>
+          <t>2,475</t>
+        </is>
+      </c>
+      <c r="C2392" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="D2392" t="inlineStr">
+        <is>
+          <t>+2.10%</t>
+        </is>
+      </c>
+      <c r="E2392" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2392" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2393">
+      <c r="A2393" t="inlineStr">
+        <is>
+          <t>현대일렉트릭</t>
+        </is>
+      </c>
+      <c r="B2393" t="inlineStr">
+        <is>
+          <t>4,117</t>
+        </is>
+      </c>
+      <c r="C2393" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="D2393" t="inlineStr">
+        <is>
+          <t>-0.52%</t>
+        </is>
+      </c>
+      <c r="E2393" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2393" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2394">
+      <c r="A2394" t="inlineStr">
+        <is>
+          <t>한온시스템</t>
+        </is>
+      </c>
+      <c r="B2394" t="inlineStr">
+        <is>
+          <t>2,458</t>
+        </is>
+      </c>
+      <c r="C2394" t="inlineStr">
+        <is>
+          <t>309</t>
+        </is>
+      </c>
+      <c r="D2394" t="inlineStr">
+        <is>
+          <t>+5.17%</t>
+        </is>
+      </c>
+      <c r="E2394" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2394" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2395">
+      <c r="A2395" t="inlineStr">
+        <is>
+          <t>DB하이텍</t>
+        </is>
+      </c>
+      <c r="B2395" t="inlineStr">
+        <is>
+          <t>3,849</t>
+        </is>
+      </c>
+      <c r="C2395" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="D2395" t="inlineStr">
+        <is>
+          <t>+3.34%</t>
+        </is>
+      </c>
+      <c r="E2395" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2395" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2396">
+      <c r="A2396" t="inlineStr">
+        <is>
+          <t>대한유화</t>
+        </is>
+      </c>
+      <c r="B2396" t="inlineStr">
+        <is>
+          <t>2,351</t>
+        </is>
+      </c>
+      <c r="C2396" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D2396" t="inlineStr">
+        <is>
+          <t>+2.53%</t>
+        </is>
+      </c>
+      <c r="E2396" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2396" t="inlineStr">
+        <is>
+          <t>2022-11-10</t>
         </is>
       </c>
     </row>

</xml_diff>